<commit_message>
No point in trying to find reference table at the end, just translate all references.
</commit_message>
<xml_diff>
--- a/MP69Equivalents.xlsx
+++ b/MP69Equivalents.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Max\Desktop\MarioParty69Java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4870D93-68C8-4746-AFA4-F54C9956272F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5156D97-6F4C-48D0-9E40-86A6C3DD77DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EB0D05C6-5931-48AA-8F53-EB8D485F66F4}"/>
+    <workbookView xWindow="8955" yWindow="225" windowWidth="8475" windowHeight="15120" xr2:uid="{EB0D05C6-5931-48AA-8F53-EB8D485F66F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="254">
   <si>
     <t>mp7 reference</t>
   </si>
@@ -780,6 +780,24 @@
   </si>
   <si>
     <t>800262f0</t>
+  </si>
+  <si>
+    <t>800A0738</t>
+  </si>
+  <si>
+    <t>800A68CC</t>
+  </si>
+  <si>
+    <t>800A08D4</t>
+  </si>
+  <si>
+    <t>800A6A68</t>
+  </si>
+  <si>
+    <t>8006AD08</t>
+  </si>
+  <si>
+    <t>8006EDB4</t>
   </si>
 </sst>
 </file>
@@ -867,6 +885,7 @@
         <family val="3"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -886,7 +905,6 @@
         <family val="3"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -923,11 +941,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{886CD958-0F04-4514-BC66-130BF7E74800}" name="Table1" displayName="Table1" ref="A1:B132" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
-  <autoFilter ref="A1:B132" xr:uid="{8C36E61F-68EE-44B6-B773-76A7B6ADFE00}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{886CD958-0F04-4514-BC66-130BF7E74800}" name="Table1" displayName="Table1" ref="A1:B135" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
+  <autoFilter ref="A1:B135" xr:uid="{8C36E61F-68EE-44B6-B773-76A7B6ADFE00}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B132">
+    <sortCondition ref="A1:A132"/>
+  </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{1773728D-161D-433F-A6F8-351ECEAD1468}" name="mp6 reference" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{D34C955A-D93A-40A9-9C67-92FE8F88D4FC}" name="mp7 reference" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{1773728D-161D-433F-A6F8-351ECEAD1468}" name="mp6 reference" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{D34C955A-D93A-40A9-9C67-92FE8F88D4FC}" name="mp7 reference" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1232,8 +1253,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D5AD9A1-E048-4F9F-8202-7E7D3A2CB996}">
   <dimension ref="A1:E566"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
+      <selection activeCell="C120" sqref="C120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1252,311 +1273,311 @@
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>244</v>
+      <c r="A2" s="1">
+        <v>80023308</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>245</v>
+        <v>95</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="B3" s="1">
-        <v>80041774</v>
+      <c r="A3" s="1">
+        <v>80026760</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>108</v>
+      <c r="A4" s="1">
+        <v>80027884</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>2</v>
+        <v>93</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>3</v>
+      <c r="A5" s="1">
+        <v>80028630</v>
+      </c>
+      <c r="B5" s="1">
+        <v>80029350</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>110</v>
+      <c r="A6" s="1">
+        <v>80099728</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>4</v>
+        <v>88</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>111</v>
+      <c r="A7" s="1">
+        <v>80099788</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>5</v>
+        <v>97</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B9" s="1">
-        <v>80028494</v>
+        <v>140</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>114</v>
+        <v>133</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B11" s="1">
-        <v>80028648</v>
+        <v>139</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>116</v>
+        <v>142</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>117</v>
+        <v>137</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>118</v>
+        <v>138</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>221</v>
+        <v>29</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>80028630</v>
-      </c>
-      <c r="B15" s="1">
-        <v>80029350</v>
+      <c r="A15" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>221</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>119</v>
+        <v>149</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B17" s="1">
-        <v>80029830</v>
+        <v>129</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>123</v>
+        <v>202</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>13</v>
+        <v>94</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>124</v>
+        <v>222</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>14</v>
+        <v>222</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>125</v>
+        <v>206</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>15</v>
+        <v>220</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>16</v>
+        <v>147</v>
+      </c>
+      <c r="B23" s="1">
+        <v>80023450</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>127</v>
+        <v>145</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>18</v>
+        <v>211</v>
+      </c>
+      <c r="B25" s="1">
+        <v>80023680</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>129</v>
+        <v>246</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>19</v>
+        <v>247</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>131</v>
+        <v>241</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>21</v>
+        <v>226</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>22</v>
+        <v>136</v>
+      </c>
+      <c r="B29" s="1">
+        <v>80027364</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>133</v>
+        <v>201</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>23</v>
+        <v>92</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>24</v>
+        <v>203</v>
+      </c>
+      <c r="B31" s="1">
+        <v>80027774</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
-        <v>80026760</v>
+      <c r="A32" s="1" t="s">
+        <v>218</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
@@ -1573,1009 +1594,1021 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>136</v>
+        <v>113</v>
       </c>
       <c r="B34" s="1">
-        <v>80027364</v>
+        <v>80028494</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>218</v>
+        <v>114</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>28</v>
+        <v>115</v>
+      </c>
+      <c r="B36" s="1">
+        <v>80028648</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>138</v>
+        <v>234</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>29</v>
+        <v>229</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>30</v>
+        <v>120</v>
+      </c>
+      <c r="B38" s="1">
+        <v>80029830</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>140</v>
+        <v>119</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>144</v>
+        <v>183</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>35</v>
+        <v>73</v>
       </c>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>146</v>
+        <v>205</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>37</v>
+        <v>219</v>
       </c>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="B46" s="1">
-        <v>80023450</v>
+        <v>128</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>148</v>
+        <v>109</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>149</v>
+        <v>117</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>39</v>
+        <v>9</v>
       </c>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>150</v>
+        <v>116</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>41</v>
+        <v>243</v>
+      </c>
+      <c r="B50" s="1">
+        <v>80041774</v>
       </c>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>152</v>
+        <v>204</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>42</v>
+        <v>96</v>
       </c>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>153</v>
+        <v>124</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>154</v>
+        <v>125</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>155</v>
+        <v>121</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>45</v>
+        <v>11</v>
       </c>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>156</v>
+        <v>240</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>46</v>
+        <v>225</v>
       </c>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>157</v>
+        <v>242</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>47</v>
+        <v>227</v>
       </c>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>158</v>
+        <v>235</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>48</v>
+        <v>223</v>
       </c>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>159</v>
+        <v>238</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>49</v>
+        <v>232</v>
       </c>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>160</v>
+        <v>233</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>50</v>
+        <v>228</v>
       </c>
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>161</v>
+        <v>236</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>51</v>
+        <v>230</v>
       </c>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>162</v>
+        <v>237</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>52</v>
+        <v>231</v>
       </c>
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>163</v>
+        <v>239</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>53</v>
+        <v>224</v>
       </c>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>165</v>
+        <v>108</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>166</v>
+        <v>191</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>56</v>
+        <v>81</v>
       </c>
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>168</v>
+        <v>209</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>58</v>
+        <v>100</v>
       </c>
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>169</v>
+        <v>144</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>171</v>
+        <v>207</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>61</v>
+        <v>98</v>
       </c>
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>173</v>
+        <v>190</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>174</v>
+        <v>244</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>64</v>
+        <v>245</v>
       </c>
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>176</v>
+        <v>155</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>66</v>
+        <v>45</v>
       </c>
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D76" s="1"/>
       <c r="E76" s="1"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="D78" s="1"/>
       <c r="E78" s="1"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="D79" s="1"/>
       <c r="E79" s="1"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D80" s="1"/>
       <c r="E80" s="1"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D81" s="1"/>
       <c r="E81" s="1"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="D82" s="1"/>
       <c r="E82" s="1"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>184</v>
+        <v>217</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>74</v>
+        <v>107</v>
       </c>
       <c r="D83" s="1"/>
       <c r="E83" s="1"/>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="D84" s="1"/>
       <c r="E84" s="1"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>186</v>
+        <v>141</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>76</v>
+        <v>32</v>
       </c>
       <c r="D85" s="1"/>
       <c r="E85" s="1"/>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D86" s="1"/>
       <c r="E86" s="1"/>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>188</v>
+        <v>200</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="D87" s="1"/>
       <c r="E87" s="1"/>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D88" s="1"/>
       <c r="E88" s="1"/>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D89" s="1"/>
       <c r="E89" s="1"/>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="D90" s="1"/>
       <c r="E90" s="1"/>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="D91" s="1"/>
       <c r="E91" s="1"/>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>193</v>
+        <v>215</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>83</v>
+        <v>105</v>
       </c>
       <c r="D92" s="1"/>
       <c r="E92" s="1"/>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>194</v>
+        <v>213</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>84</v>
+        <v>103</v>
       </c>
       <c r="D93" s="1"/>
       <c r="E93" s="1"/>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>195</v>
+        <v>212</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>85</v>
+        <v>102</v>
       </c>
       <c r="D94" s="1"/>
       <c r="E94" s="1"/>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>196</v>
+        <v>216</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="D95" s="1"/>
       <c r="E95" s="1"/>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>197</v>
+        <v>214</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
       <c r="D96" s="1"/>
       <c r="E96" s="1"/>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A97" s="1">
-        <v>80099728</v>
+      <c r="A97" s="1" t="s">
+        <v>174</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="D97" s="1"/>
       <c r="E97" s="1"/>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>198</v>
+        <v>176</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>89</v>
+        <v>66</v>
       </c>
       <c r="D98" s="1"/>
       <c r="E98" s="1"/>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>199</v>
+        <v>175</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>90</v>
+        <v>65</v>
       </c>
       <c r="D99" s="1"/>
       <c r="E99" s="1"/>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>200</v>
+        <v>177</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="D100" s="1"/>
       <c r="E100" s="1"/>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="D101" s="1"/>
       <c r="E101" s="1"/>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A102" s="1">
-        <v>80027884</v>
+      <c r="A102" s="1" t="s">
+        <v>195</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D102" s="1"/>
       <c r="E102" s="1"/>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="D103" s="1"/>
       <c r="E103" s="1"/>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="B104" s="1">
-        <v>80027774</v>
+        <v>193</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>83</v>
       </c>
       <c r="D104" s="1"/>
       <c r="E104" s="1"/>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A105" s="1">
-        <v>80023308</v>
+      <c r="A105" s="1" t="s">
+        <v>173</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>95</v>
+        <v>63</v>
       </c>
       <c r="D105" s="1"/>
       <c r="E105" s="1"/>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>204</v>
+        <v>180</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>96</v>
+        <v>70</v>
       </c>
       <c r="D106" s="1"/>
       <c r="E106" s="1"/>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A107" s="1">
-        <v>80099788</v>
+      <c r="A107" s="1" t="s">
+        <v>182</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>97</v>
+        <v>72</v>
       </c>
       <c r="D107" s="1"/>
       <c r="E107" s="1"/>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>205</v>
+        <v>181</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>219</v>
+        <v>71</v>
       </c>
       <c r="D108" s="1"/>
       <c r="E108" s="1"/>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>206</v>
+        <v>164</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>220</v>
+        <v>54</v>
       </c>
       <c r="D109" s="1"/>
       <c r="E109" s="1"/>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>207</v>
+        <v>168</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>98</v>
+        <v>58</v>
       </c>
       <c r="D110" s="1"/>
       <c r="E110" s="1"/>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D111" s="1"/>
       <c r="E111" s="1"/>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>209</v>
+        <v>165</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>100</v>
+        <v>55</v>
       </c>
       <c r="D112" s="1"/>
       <c r="E112" s="1"/>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>210</v>
+        <v>166</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>101</v>
+        <v>56</v>
       </c>
       <c r="D113" s="1"/>
       <c r="E113" s="1"/>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="B114" s="1">
-        <v>80023680</v>
+        <v>154</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="D114" s="1"/>
       <c r="E114" s="1"/>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>212</v>
+        <v>146</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>102</v>
+        <v>37</v>
       </c>
       <c r="D115" s="1"/>
       <c r="E115" s="1"/>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>213</v>
+        <v>188</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>103</v>
+        <v>78</v>
       </c>
       <c r="D116" s="1"/>
       <c r="E116" s="1"/>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>214</v>
+        <v>197</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>104</v>
+        <v>87</v>
       </c>
       <c r="D117" s="1"/>
       <c r="E117" s="1"/>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
       <c r="D118" s="1"/>
       <c r="E118" s="1"/>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>216</v>
+        <v>162</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>106</v>
+        <v>52</v>
       </c>
       <c r="D119" s="1"/>
       <c r="E119" s="1"/>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="D120" s="1"/>
       <c r="E120" s="1"/>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>222</v>
+        <v>110</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>222</v>
+        <v>4</v>
       </c>
       <c r="D121" s="1"/>
       <c r="E121" s="1"/>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>233</v>
+        <v>111</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>228</v>
+        <v>5</v>
       </c>
       <c r="D122" s="1"/>
       <c r="E122" s="1"/>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>234</v>
+        <v>153</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>229</v>
+        <v>43</v>
       </c>
       <c r="D123" s="1"/>
       <c r="E123" s="1"/>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>235</v>
+        <v>152</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>223</v>
+        <v>42</v>
       </c>
       <c r="D124" s="1"/>
       <c r="E124" s="1"/>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>236</v>
+        <v>158</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>230</v>
+        <v>48</v>
       </c>
       <c r="D125" s="1"/>
       <c r="E125" s="1"/>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>237</v>
+        <v>157</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>231</v>
+        <v>47</v>
       </c>
       <c r="D126" s="1"/>
       <c r="E126" s="1"/>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>238</v>
+        <v>150</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>232</v>
+        <v>40</v>
       </c>
       <c r="D127" s="1"/>
       <c r="E127" s="1"/>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>239</v>
+        <v>151</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>224</v>
+        <v>41</v>
       </c>
       <c r="D128" s="1"/>
       <c r="E128" s="1"/>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>240</v>
+        <v>126</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>225</v>
+        <v>16</v>
       </c>
       <c r="D129" s="1"/>
       <c r="E129" s="1"/>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>241</v>
+        <v>159</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>226</v>
+        <v>49</v>
       </c>
       <c r="D130" s="1"/>
       <c r="E130" s="1"/>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>242</v>
+        <v>161</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>227</v>
+        <v>51</v>
       </c>
       <c r="D131" s="1"/>
       <c r="E131" s="1"/>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>246</v>
+        <v>112</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>247</v>
+        <v>6</v>
       </c>
       <c r="D132" s="1"/>
       <c r="E132" s="1"/>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A133"/>
-      <c r="B133"/>
+      <c r="A133" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>249</v>
+      </c>
       <c r="D133" s="1"/>
       <c r="E133" s="1"/>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A134"/>
-      <c r="B134"/>
+      <c r="A134" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>251</v>
+      </c>
       <c r="D134" s="1"/>
       <c r="E134" s="1"/>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A135"/>
-      <c r="B135"/>
+      <c r="A135" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>253</v>
+      </c>
       <c r="D135" s="1"/>
       <c r="E135" s="1"/>
     </row>

</xml_diff>